<commit_message>
now uses random k walks
</commit_message>
<xml_diff>
--- a/graphs/homogeneity_results.xlsx
+++ b/graphs/homogeneity_results.xlsx
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:13</t>
+          <t>2025-06-30 15:52:22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -511,16 +511,16 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1120305471122265</v>
+        <v>0.4062295250005263</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001867175785203775</v>
+        <v>0.006770492083342105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:13</t>
+          <t>2025-06-30 15:52:24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -548,16 +548,16 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.08171798288822174</v>
+        <v>0.8164158939998742</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001361966381470362</v>
+        <v>0.01360693156666457</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:14</t>
+          <t>2025-06-30 15:52:28</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -585,16 +585,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5111126564443111</v>
+        <v>1.612165862001348</v>
       </c>
       <c r="I4" t="n">
-        <v>0.008518544274071853</v>
+        <v>0.0268694310333558</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:15</t>
+          <t>2025-06-30 15:52:32</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -622,16 +622,16 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5368059240281582</v>
+        <v>2.297024873998453</v>
       </c>
       <c r="I5" t="n">
-        <v>0.008946765400469302</v>
+        <v>0.03828374789997421</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:15</t>
+          <t>2025-06-30 15:52:34</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -659,16 +659,16 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4957016967236996</v>
+        <v>1.507214932000352</v>
       </c>
       <c r="I6" t="n">
-        <v>0.008261694945394993</v>
+        <v>0.02512024886667253</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:16</t>
+          <t>2025-06-30 15:52:36</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -696,16 +696,16 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.518499743193388</v>
+        <v>1.644610892999481</v>
       </c>
       <c r="I7" t="n">
-        <v>0.008641662386556467</v>
+        <v>0.02741018154999135</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:16</t>
+          <t>2025-06-30 15:52:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -733,16 +733,16 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1236398667097092</v>
+        <v>0.5215015570011019</v>
       </c>
       <c r="I8" t="n">
-        <v>0.00206066444516182</v>
+        <v>0.008691692616685032</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:17</t>
+          <t>2025-06-30 15:52:41</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -770,16 +770,16 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.09444002062082291</v>
+        <v>0.6393786439984979</v>
       </c>
       <c r="I9" t="n">
-        <v>0.001574000343680382</v>
+        <v>0.0106563107333083</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:17</t>
+          <t>2025-06-30 15:52:42</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -807,16 +807,16 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0942070446908474</v>
+        <v>0.5050186199987365</v>
       </c>
       <c r="I10" t="n">
-        <v>0.001570117411514123</v>
+        <v>0.008416976999978943</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:17</t>
+          <t>2025-06-30 15:52:43</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -844,16 +844,16 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.09458367526531219</v>
+        <v>0.7903485089991591</v>
       </c>
       <c r="I11" t="n">
-        <v>0.001576394587755203</v>
+        <v>0.01317247514998598</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:18</t>
+          <t>2025-06-30 15:52:45</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -881,16 +881,16 @@
         <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>1.147807572036982</v>
+        <v>2.478934319999098</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01913012620061636</v>
+        <v>0.04131557199998497</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:19</t>
+          <t>2025-06-30 15:52:48</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -918,16 +918,16 @@
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>1.192090682685375</v>
+        <v>2.244191810001212</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01986817804475625</v>
+        <v>0.03740319683335353</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:20</t>
+          <t>2025-06-30 15:52:48</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -955,16 +955,16 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2715951502323151</v>
+        <v>0.6502726430007897</v>
       </c>
       <c r="I14" t="n">
-        <v>0.004526585837205251</v>
+        <v>0.01083787738334649</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:20</t>
+          <t>2025-06-30 15:52:49</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -992,16 +992,16 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2258936017751694</v>
+        <v>1.002967914000692</v>
       </c>
       <c r="I15" t="n">
-        <v>0.00376489336291949</v>
+        <v>0.01671613190001153</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:20</t>
+          <t>2025-06-30 15:52:50</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1029,16 +1029,16 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2282694131135941</v>
+        <v>0.5895341870000266</v>
       </c>
       <c r="I16" t="n">
-        <v>0.003804490218559901</v>
+        <v>0.009825569783333776</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:21</t>
+          <t>2025-06-30 15:52:51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1066,16 +1066,16 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2295455746352673</v>
+        <v>0.8703951299994515</v>
       </c>
       <c r="I17" t="n">
-        <v>0.003825759577254454</v>
+        <v>0.01450658549999086</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:24</t>
+          <t>2025-06-30 15:52:57</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1103,16 +1103,16 @@
         <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>3.525264862924814</v>
+        <v>5.722113347999766</v>
       </c>
       <c r="I18" t="n">
-        <v>0.05875441438208024</v>
+        <v>0.0953685557999961</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:28</t>
+          <t>2025-06-30 15:53:05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1140,16 +1140,16 @@
         <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>3.537259321659803</v>
+        <v>7.568989397001133</v>
       </c>
       <c r="I19" t="n">
-        <v>0.05895432202766339</v>
+        <v>0.1261498232833522</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:29</t>
+          <t>2025-06-30 15:53:07</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1177,16 +1177,16 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1.440809901803732</v>
+        <v>2.219762081000226</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02401349836339553</v>
+        <v>0.03699603468333711</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:31</t>
+          <t>2025-06-30 15:53:10</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1214,16 +1214,16 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>1.491383697837591</v>
+        <v>2.54578781499913</v>
       </c>
       <c r="I21" t="n">
-        <v>0.02485639496395985</v>
+        <v>0.04242979691665217</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:32</t>
+          <t>2025-06-30 15:53:16</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1251,16 +1251,16 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>1.426564015448093</v>
+        <v>5.39196689200071</v>
       </c>
       <c r="I22" t="n">
-        <v>0.02377606692413489</v>
+        <v>0.08986611486667849</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-06-30 01:56:34</t>
+          <t>2025-06-30 15:53:21</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1288,16 +1288,16 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>1.431711550801992</v>
+        <v>4.75843328999872</v>
       </c>
       <c r="I23" t="n">
-        <v>0.02386185918003321</v>
+        <v>0.07930722149997867</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:01</t>
+          <t>2025-06-30 15:54:09</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1325,16 +1325,16 @@
         <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>27.30860134586692</v>
+        <v>47.45290445399951</v>
       </c>
       <c r="I24" t="n">
-        <v>0.4551433557644486</v>
+        <v>0.7908817408999919</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:28</t>
+          <t>2025-06-30 15:55:09</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1362,16 +1362,16 @@
         <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>27.25011755526066</v>
+        <v>58.70256671199968</v>
       </c>
       <c r="I25" t="n">
-        <v>0.454168625921011</v>
+        <v>0.9783761118666613</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:29</t>
+          <t>2025-06-30 15:55:11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1399,16 +1399,16 @@
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1310737058520317</v>
+        <v>1.179922424998949</v>
       </c>
       <c r="I26" t="n">
-        <v>0.002184561764200529</v>
+        <v>0.01966537374998249</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:29</t>
+          <t>2025-06-30 15:55:13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1436,16 +1436,16 @@
         <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0.109433688223362</v>
+        <v>1.215688584999953</v>
       </c>
       <c r="I27" t="n">
-        <v>0.001823894803722699</v>
+        <v>0.02026147641666588</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:29</t>
+          <t>2025-06-30 15:55:15</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1473,16 +1473,16 @@
         <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>0.5704975314438343</v>
+        <v>1.916633518998424</v>
       </c>
       <c r="I28" t="n">
-        <v>0.009508292190730572</v>
+        <v>0.03194389198330706</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:30</t>
+          <t>2025-06-30 15:55:18</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1510,16 +1510,16 @@
         <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>0.6097546182572842</v>
+        <v>1.772929955999643</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01016257697095474</v>
+        <v>0.02954883259999406</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:30</t>
+          <t>2025-06-30 15:55:19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1547,16 +1547,16 @@
         <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>0.6128988564014435</v>
+        <v>1.222169370998017</v>
       </c>
       <c r="I30" t="n">
-        <v>0.01021498094002406</v>
+        <v>0.02036948951663362</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:31</t>
+          <t>2025-06-30 15:55:21</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1584,16 +1584,16 @@
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>0.6125242672860622</v>
+        <v>1.496579381000629</v>
       </c>
       <c r="I31" t="n">
-        <v>0.01020873778810104</v>
+        <v>0.02494298968334381</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:31</t>
+          <t>2025-06-30 15:55:22</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1621,16 +1621,16 @@
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.1185627542436123</v>
+        <v>1.093284569999014</v>
       </c>
       <c r="I32" t="n">
-        <v>0.001976045904060205</v>
+        <v>0.01822140949998357</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:31</t>
+          <t>2025-06-30 15:55:24</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1658,16 +1658,16 @@
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1478199623525143</v>
+        <v>1.455271278999135</v>
       </c>
       <c r="I33" t="n">
-        <v>0.002463666039208571</v>
+        <v>0.02425452131665224</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:32</t>
+          <t>2025-06-30 15:55:25</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1695,16 +1695,16 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0.3418194688856602</v>
+        <v>1.670620955999766</v>
       </c>
       <c r="I34" t="n">
-        <v>0.005696991148094336</v>
+        <v>0.0278436825999961</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:32</t>
+          <t>2025-06-30 15:55:28</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1729,19 +1729,19 @@
         <v>5500</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0.3223056234419346</v>
+        <v>2.83374197899866</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00537176039069891</v>
+        <v>0.047229032983311</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:33</t>
+          <t>2025-06-30 15:55:32</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1769,16 +1769,16 @@
         <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>1.24194260686636</v>
+        <v>3.907361851999667</v>
       </c>
       <c r="I36" t="n">
-        <v>0.02069904344777266</v>
+        <v>0.06512269753332779</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:35</t>
+          <t>2025-06-30 15:55:36</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1806,16 +1806,16 @@
         <v>1</v>
       </c>
       <c r="H37" t="n">
-        <v>1.284206286072731</v>
+        <v>3.392312944999503</v>
       </c>
       <c r="I37" t="n">
-        <v>0.02140343810121218</v>
+        <v>0.05653854908332505</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:35</t>
+          <t>2025-06-30 15:55:37</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1843,16 +1843,16 @@
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>0.432347733527422</v>
+        <v>1.009835412998655</v>
       </c>
       <c r="I38" t="n">
-        <v>0.007205795558790366</v>
+        <v>0.01683059021664424</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:35</t>
+          <t>2025-06-30 15:55:38</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1880,16 +1880,16 @@
         <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>0.424174752086401</v>
+        <v>0.9598234920013056</v>
       </c>
       <c r="I39" t="n">
-        <v>0.007069579201440016</v>
+        <v>0.01599705820002176</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:36</t>
+          <t>2025-06-30 15:55:39</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1917,16 +1917,16 @@
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0.4162007458508015</v>
+        <v>0.8452638460003072</v>
       </c>
       <c r="I40" t="n">
-        <v>0.006936679097513358</v>
+        <v>0.01408773076667179</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:36</t>
+          <t>2025-06-30 15:55:40</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1954,16 +1954,16 @@
         <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0.4319259524345398</v>
+        <v>0.6424764350012993</v>
       </c>
       <c r="I41" t="n">
-        <v>0.007198765873908997</v>
+        <v>0.01070794058335499</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:41</t>
+          <t>2025-06-30 15:55:59</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1991,16 +1991,16 @@
         <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>4.734641082584858</v>
+        <v>18.85149766399991</v>
       </c>
       <c r="I42" t="n">
-        <v>0.07891068470974763</v>
+        <v>0.3141916277333318</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:46</t>
+          <t>2025-06-30 15:56:12</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2028,16 +2028,16 @@
         <v>1</v>
       </c>
       <c r="H43" t="n">
-        <v>4.704186365008354</v>
+        <v>12.08913742199911</v>
       </c>
       <c r="I43" t="n">
-        <v>0.07840310608347258</v>
+        <v>0.2014856236999852</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:48</t>
+          <t>2025-06-30 15:56:19</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2065,16 +2065,16 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>2.112755283713341</v>
+        <v>7.685707819000527</v>
       </c>
       <c r="I44" t="n">
-        <v>0.03521258806188901</v>
+        <v>0.1280951303166754</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:50</t>
+          <t>2025-06-30 15:56:28</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2102,16 +2102,16 @@
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>2.040099240839481</v>
+        <v>7.764954210000724</v>
       </c>
       <c r="I45" t="n">
-        <v>0.03400165401399136</v>
+        <v>0.1294159035000121</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:52</t>
+          <t>2025-06-30 15:56:33</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2139,16 +2139,16 @@
         <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>2.031102042645216</v>
+        <v>5.009041246999914</v>
       </c>
       <c r="I46" t="n">
-        <v>0.0338517007107536</v>
+        <v>0.08348402078333189</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-06-30 01:57:54</t>
+          <t>2025-06-30 15:56:38</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2176,16 +2176,16 @@
         <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>2.032477177679539</v>
+        <v>4.832566375001988</v>
       </c>
       <c r="I47" t="n">
-        <v>0.03387461962799231</v>
+        <v>0.08054277291669981</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:25</t>
+          <t>2025-06-30 15:57:30</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2213,16 +2213,16 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>31.00024297460914</v>
+        <v>50.04493833900051</v>
       </c>
       <c r="I48" t="n">
-        <v>0.5166707162434856</v>
+        <v>0.8340823056500085</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:56</t>
+          <t>2025-06-30 15:58:07</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2250,16 +2250,16 @@
         <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>30.79569852352142</v>
+        <v>36.67295894500057</v>
       </c>
       <c r="I49" t="n">
-        <v>0.5132616420586904</v>
+        <v>0.6112159824166762</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:56</t>
+          <t>2025-06-30 15:58:08</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2287,16 +2287,16 @@
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>0.3412343934178352</v>
+        <v>0.4599636949988053</v>
       </c>
       <c r="I50" t="n">
-        <v>0.005687239890297254</v>
+        <v>0.007666061583313422</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:57</t>
+          <t>2025-06-30 15:58:09</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2321,19 +2321,19 @@
         <v>3500</v>
       </c>
       <c r="G51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
-        <v>0.3176261335611343</v>
+        <v>0.8154324669976631</v>
       </c>
       <c r="I51" t="n">
-        <v>0.005293768892685572</v>
+        <v>0.01359054111662772</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:57</t>
+          <t>2025-06-30 15:58:10</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2361,16 +2361,16 @@
         <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>0.5966770015656948</v>
+        <v>0.6895937379995303</v>
       </c>
       <c r="I52" t="n">
-        <v>0.009944616692761581</v>
+        <v>0.01149322896665884</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:58</t>
+          <t>2025-06-30 15:58:11</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2398,16 +2398,16 @@
         <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>0.6024949550628662</v>
+        <v>0.7418875459989067</v>
       </c>
       <c r="I53" t="n">
-        <v>0.0100415825843811</v>
+        <v>0.01236479243331511</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:59</t>
+          <t>2025-06-30 15:58:11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2435,16 +2435,16 @@
         <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>0.5987833477556705</v>
+        <v>0.9254292019977584</v>
       </c>
       <c r="I54" t="n">
-        <v>0.009979722462594509</v>
+        <v>0.01542382003329597</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:59</t>
+          <t>2025-06-30 15:58:12</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2472,16 +2472,16 @@
         <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>0.6006513722240925</v>
+        <v>0.797318651999376</v>
       </c>
       <c r="I55" t="n">
-        <v>0.01001085620373487</v>
+        <v>0.0132886441999896</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-06-30 01:58:59</t>
+          <t>2025-06-30 15:58:13</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2509,16 +2509,16 @@
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0.2400498017668724</v>
+        <v>0.3889139940001769</v>
       </c>
       <c r="I56" t="n">
-        <v>0.004000830029447873</v>
+        <v>0.006481899900002948</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:00</t>
+          <t>2025-06-30 15:58:14</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2546,16 +2546,16 @@
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0.2214519530534744</v>
+        <v>0.8342936650005868</v>
       </c>
       <c r="I57" t="n">
-        <v>0.003690865884224574</v>
+        <v>0.01390489441667645</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:00</t>
+          <t>2025-06-30 15:58:17</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2580,19 +2580,19 @@
         <v>5000</v>
       </c>
       <c r="G58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>0.2940305098891258</v>
+        <v>3.20689770700119</v>
       </c>
       <c r="I58" t="n">
-        <v>0.004900508498152097</v>
+        <v>0.05344829511668649</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:01</t>
+          <t>2025-06-30 15:58:20</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2620,16 +2620,16 @@
         <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>1.334041956812143</v>
+        <v>2.601533756000208</v>
       </c>
       <c r="I59" t="n">
-        <v>0.02223403261353572</v>
+        <v>0.0433588959333368</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:03</t>
+          <t>2025-06-30 15:58:22</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2657,16 +2657,16 @@
         <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>1.344309989362955</v>
+        <v>1.549130015000628</v>
       </c>
       <c r="I60" t="n">
-        <v>0.02240516648938258</v>
+        <v>0.0258188335833438</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:04</t>
+          <t>2025-06-30 15:58:24</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2694,16 +2694,16 @@
         <v>1</v>
       </c>
       <c r="H61" t="n">
-        <v>1.351344797760248</v>
+        <v>2.242114954000499</v>
       </c>
       <c r="I61" t="n">
-        <v>0.02252241329600414</v>
+        <v>0.03736858256667498</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:04</t>
+          <t>2025-06-30 15:58:25</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2731,16 +2731,16 @@
         <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>0.282353650778532</v>
+        <v>0.4932124640017719</v>
       </c>
       <c r="I62" t="n">
-        <v>0.004705894179642201</v>
+        <v>0.008220207733362865</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:05</t>
+          <t>2025-06-30 15:58:25</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2768,16 +2768,16 @@
         <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>0.2647651582956314</v>
+        <v>0.5108637730027112</v>
       </c>
       <c r="I63" t="n">
-        <v>0.004412752638260523</v>
+        <v>0.008514396216711854</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:05</t>
+          <t>2025-06-30 15:58:26</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2805,16 +2805,16 @@
         <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>0.2734615840017796</v>
+        <v>0.4465496490010992</v>
       </c>
       <c r="I64" t="n">
-        <v>0.004557693066696326</v>
+        <v>0.00744249415001832</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:05</t>
+          <t>2025-06-30 15:58:26</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2842,16 +2842,16 @@
         <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>0.2897685058414936</v>
+        <v>0.3498728820013639</v>
       </c>
       <c r="I65" t="n">
-        <v>0.004829475097358227</v>
+        <v>0.005831214700022732</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:10</t>
+          <t>2025-06-30 15:58:34</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2879,16 +2879,16 @@
         <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>4.594378858804703</v>
+        <v>7.067512942001485</v>
       </c>
       <c r="I66" t="n">
-        <v>0.07657298098007838</v>
+        <v>0.1177918823666914</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:14</t>
+          <t>2025-06-30 15:58:44</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2916,16 +2916,16 @@
         <v>1</v>
       </c>
       <c r="H67" t="n">
-        <v>4.647321410477161</v>
+        <v>9.75605522600199</v>
       </c>
       <c r="I67" t="n">
-        <v>0.07745535684128603</v>
+        <v>0.1626009204333665</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:17</t>
+          <t>2025-06-30 15:58:50</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2953,16 +2953,16 @@
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>2.039279267191887</v>
+        <v>6.055649170000834</v>
       </c>
       <c r="I68" t="n">
-        <v>0.03398798778653145</v>
+        <v>0.1009274861666806</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:19</t>
+          <t>2025-06-30 15:58:55</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2990,16 +2990,16 @@
         <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>1.969639584422112</v>
+        <v>4.742074251002123</v>
       </c>
       <c r="I69" t="n">
-        <v>0.03282732640703519</v>
+        <v>0.07903457085003537</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:21</t>
+          <t>2025-06-30 15:59:00</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3027,16 +3027,16 @@
         <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>1.984736390411854</v>
+        <v>4.798819904000993</v>
       </c>
       <c r="I70" t="n">
-        <v>0.03307893984019757</v>
+        <v>0.07998033173334988</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:23</t>
+          <t>2025-06-30 15:59:05</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3064,16 +3064,16 @@
         <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>1.987357251346111</v>
+        <v>5.11635772000227</v>
       </c>
       <c r="I71" t="n">
-        <v>0.03312262085576852</v>
+        <v>0.0852726286667045</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:33</t>
+          <t>2025-06-30 15:59:11</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3101,16 +3101,16 @@
         <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>10.66459095478058</v>
+        <v>4.606829291002214</v>
       </c>
       <c r="I72" t="n">
-        <v>0.1777431825796763</v>
+        <v>0.07678048818337023</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-06-30 01:59:51</t>
+          <t>2025-06-30 15:59:33</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3138,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>17.24615224078298</v>
+        <v>22.60443701400072</v>
       </c>
       <c r="I73" t="n">
-        <v>0.2874358706797163</v>
+        <v>0.376740616900012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to use both modes hybrid and direct
</commit_message>
<xml_diff>
--- a/graphs/homogeneity_results.xlsx
+++ b/graphs/homogeneity_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-07-01 23:37:06</t>
+          <t>2025-07-01 23:52:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -511,16 +511,16 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5386378989933291</v>
+        <v>0.2879897669990896</v>
       </c>
       <c r="I2" t="n">
-        <v>0.008977298316555487</v>
+        <v>0.004799829449984827</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-07-01 23:37:07</t>
+          <t>2025-07-01 23:52:35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -548,16 +548,16 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5101022279995959</v>
+        <v>0.2778664880024735</v>
       </c>
       <c r="I3" t="n">
-        <v>0.008501703799993265</v>
+        <v>0.004631108133374558</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-07-01 23:37:08</t>
+          <t>2025-07-01 23:52:39</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -585,16 +585,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1.591351128001406</v>
+        <v>4.519339108999702</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02652251880002344</v>
+        <v>0.07532231848332836</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-07-01 23:37:10</t>
+          <t>2025-07-01 23:52:45</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -622,232 +622,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>1.959665363996464</v>
+        <v>5.357828082000196</v>
       </c>
       <c r="I5" t="n">
-        <v>0.03266108939994107</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-07-01 23:37:12</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>RWUnlearning</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>{'Exercise': '3 - 4 times per week'}</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>{'RaceEthnicity': 'White or of European descent'}</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F6" t="n">
-        <v>60000</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.088530318993435</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.03480883864989058</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-07-01 23:37:14</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>RWUnlearning</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{'Exercise': '3 - 4 times per week'}</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>{'RaceEthnicity': 'White or of European descent'}</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>65000</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.814110026993148</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.03023516711655248</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-07-01 23:37:15</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>RWUnlearning</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{'Exercise': '3 - 4 times per week'}</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>{'RaceEthnicity': 'White or of European descent'}</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F8" t="n">
-        <v>3000</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.2122275720030302</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.003537126200050504</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-07-01 23:37:15</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>RWUnlearning</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{'Exercise': '3 - 4 times per week'}</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>{'RaceEthnicity': 'White or of European descent'}</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3500</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.2613827129971469</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.004356378549952448</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2025-07-01 23:37:16</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>RWUnlearning</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'Exercise': '3 - 4 times per week'}</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>{'RaceEthnicity': 'White or of European descent'}</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F10" t="n">
-        <v>5000</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1.449539927998558</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.02415899879997596</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-07-01 23:37:18</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>RWUnlearning</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{'Exercise': '3 - 4 times per week'}</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>{'RaceEthnicity': 'White or of European descent'}</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F11" t="n">
-        <v>5500</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.406749698995554</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.02344582831659257</v>
+        <v>0.08929713470000328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>